<commit_message>
Roiy and Xianguo pilot
</commit_message>
<xml_diff>
--- a/FilmFinder/FilmFinder/bin/Debug/Pilots and trials/Subject 9 - fourth pilot by paymahn.xlsx
+++ b/FilmFinder/FilmFinder/bin/Debug/Pilots and trials/Subject 9 - fourth pilot by paymahn.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Subject 9 - fourth pilot by pay" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -790,11 +790,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="206504320"/>
-        <c:axId val="206505856"/>
+        <c:axId val="96138368"/>
+        <c:axId val="96139904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="206504320"/>
+        <c:axId val="96138368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -803,7 +803,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="206505856"/>
+        <c:crossAx val="96139904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -811,7 +811,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="206505856"/>
+        <c:axId val="96139904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -822,10 +822,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="206504320"/>
+        <c:crossAx val="96138368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -1117,11 +1123,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="195394560"/>
-        <c:axId val="196301568"/>
+        <c:axId val="118595968"/>
+        <c:axId val="118597504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="195394560"/>
+        <c:axId val="118595968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1130,7 +1136,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196301568"/>
+        <c:crossAx val="118597504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1138,7 +1144,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196301568"/>
+        <c:axId val="118597504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1149,7 +1155,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195394560"/>
+        <c:crossAx val="118595968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1526,7 +1532,7 @@
   <dimension ref="A1:P72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>